<commit_message>
Switched to Com Proto
</commit_message>
<xml_diff>
--- a/code/CommProtocol/xBee_to_Platform.xlsx
+++ b/code/CommProtocol/xBee_to_Platform.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geri\Documents\GitHub\GCS\code\CommProtocol\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="8340"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>last 4 digits</t>
   </si>
@@ -106,12 +111,21 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Sidkidat</t>
+  </si>
+  <si>
+    <t>Valiant</t>
+  </si>
+  <si>
+    <t>UGV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,7 +245,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,9 +278,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,6 +330,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +576,9 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
@@ -539,6 +590,9 @@
       <c r="B5" s="1">
         <v>7974</v>
       </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
       <c r="D5">
         <v>3</v>
       </c>
@@ -560,6 +614,9 @@
       </c>
       <c r="B7" t="s">
         <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
       </c>
       <c r="D7">
         <v>5</v>

</xml_diff>